<commit_message>
Updated initial relative weighting parameter to match
</commit_message>
<xml_diff>
--- a/Testing/data/sphere/optimize.xlsx
+++ b/Testing/data/sphere/optimize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Testing/data/sphere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D185B4C-509B-E54F-9F6A-FE8B5CA319DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D76413-EBFA-8445-927B-667E6D988750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="15540" windowHeight="17460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,12 @@
     <sheet name="studio" sheetId="5" r:id="rId5"/>
     <sheet name="project" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
   <si>
     <t>segmentation_file</t>
   </si>
@@ -224,6 +224,36 @@
   </si>
   <si>
     <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -0.000149 -0.000149 -0.000149</t>
+  </si>
+  <si>
+    <t>local_particles</t>
+  </si>
+  <si>
+    <t>sphere10_DT_local.particles</t>
+  </si>
+  <si>
+    <t>world_particles</t>
+  </si>
+  <si>
+    <t>sphere10_DT_world.particles</t>
+  </si>
+  <si>
+    <t>sphere20_DT_local.particles</t>
+  </si>
+  <si>
+    <t>sphere20_DT_world.particles</t>
+  </si>
+  <si>
+    <t>sphere30_DT_local.particles</t>
+  </si>
+  <si>
+    <t>sphere30_DT_world.particles</t>
+  </si>
+  <si>
+    <t>sphere40_DT_local.particles</t>
+  </si>
+  <si>
+    <t>sphere40_DT_world.particles</t>
   </si>
 </sst>
 </file>
@@ -541,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E1048576"/>
@@ -549,7 +579,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,8 +589,14 @@
       <c r="C1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -570,8 +606,14 @@
       <c r="C2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -581,8 +623,14 @@
       <c r="C3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -592,8 +640,14 @@
       <c r="C4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -602,6 +656,12 @@
       </c>
       <c r="C5" t="s">
         <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +775,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,8 +803,8 @@
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
+      <c r="B3">
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Remove particle files from project
</commit_message>
<xml_diff>
--- a/Testing/data/sphere/optimize.xlsx
+++ b/Testing/data/sphere/optimize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Testing/data/sphere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D76413-EBFA-8445-927B-667E6D988750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28BC832-D6B9-E548-823C-636418FBD500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15540" windowHeight="17460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15540" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
   <si>
     <t>segmentation_file</t>
   </si>
@@ -224,36 +224,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -0.000149 -0.000149 -0.000149</t>
-  </si>
-  <si>
-    <t>local_particles</t>
-  </si>
-  <si>
-    <t>sphere10_DT_local.particles</t>
-  </si>
-  <si>
-    <t>world_particles</t>
-  </si>
-  <si>
-    <t>sphere10_DT_world.particles</t>
-  </si>
-  <si>
-    <t>sphere20_DT_local.particles</t>
-  </si>
-  <si>
-    <t>sphere20_DT_world.particles</t>
-  </si>
-  <si>
-    <t>sphere30_DT_local.particles</t>
-  </si>
-  <si>
-    <t>sphere30_DT_world.particles</t>
-  </si>
-  <si>
-    <t>sphere40_DT_local.particles</t>
-  </si>
-  <si>
-    <t>sphere40_DT_world.particles</t>
   </si>
 </sst>
 </file>
@@ -571,15 +541,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,14 +559,8 @@
       <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -606,14 +570,8 @@
       <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -623,14 +581,8 @@
       <c r="C3" t="s">
         <v>60</v>
       </c>
-      <c r="D3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -640,14 +592,8 @@
       <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -656,12 +602,6 @@
       </c>
       <c r="C5" t="s">
         <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -774,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>